<commit_message>
working rds output in excel sheet
</commit_message>
<xml_diff>
--- a/cloud_audit_report.xlsx
+++ b/cloud_audit_report.xlsx
@@ -13,6 +13,7 @@
     <sheet name="AMIs - Instance Store Backed" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Lambda - Functions" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="S3 - Bucket Analysis" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="RDS - Instances" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1050,12 +1051,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>ami-0c757bca3918f6fa9</t>
+          <t>ami-01b2b400e24fcdbe5</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>jitsi</t>
+          <t>jitsi-2-latest</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -1072,12 +1073,12 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>ami-0f84d671dcbc8a5e9</t>
+          <t>ami-0d1213ebe53bab3a3</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>jitsi-4</t>
+          <t>jitsi-2</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
@@ -1094,12 +1095,12 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>ami-01b2b400e24fcdbe5</t>
+          <t>ami-0eb42d6e6d10db5d1</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>jitsi-2-latest</t>
+          <t>jitsi-5</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -1116,12 +1117,12 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>ami-03fe541226ed7a78f</t>
+          <t>ami-0ef04d7a197cea5c8</t>
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>jitsi-final</t>
+          <t>jitsi-2-official</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
@@ -1138,12 +1139,12 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>ami-0eb42d6e6d10db5d1</t>
+          <t>ami-03fe541226ed7a78f</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>jitsi-5</t>
+          <t>jitsi-final</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -1160,12 +1161,12 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>ami-0d1213ebe53bab3a3</t>
+          <t>ami-0c757bca3918f6fa9</t>
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>jitsi-2</t>
+          <t>jitsi</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
@@ -1182,12 +1183,12 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>ami-0ef04d7a197cea5c8</t>
+          <t>ami-0f84d671dcbc8a5e9</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>jitsi-2-official</t>
+          <t>jitsi-4</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1382,7 +1383,7 @@
       <c r="I3" s="5" t="inlineStr"/>
       <c r="J3" s="5" t="inlineStr"/>
       <c r="K3" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L3" s="5" t="n"/>
       <c r="M3" s="5" t="n"/>
@@ -2236,4 +2237,30 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Invalid data format.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
resolved rds issue of invalid format
</commit_message>
<xml_diff>
--- a/cloud_audit_report.xlsx
+++ b/cloud_audit_report.xlsx
@@ -9,11 +9,9 @@
   <sheets>
     <sheet name="EC2 - Idle Instances" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Snapshots - Orphaned" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ENIs - Unattached" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="AMIs - Instance Store Backed" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Lambda - Functions" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="S3 - Bucket Analysis" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="RDS - Instances" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="AMIs - Instance Store Backed" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Lambda - Functions" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="S3 - Bucket Analysis" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,12 +541,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>i-06e22be674428fb8d</t>
+          <t>i-08e4ad439ae47d2f2</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>new-jitsi</t>
+          <t>jitsi</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -558,7 +556,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>2025-06-14 04:05:33+00:00</t>
+          <t>2025-06-17 09:24:23+00:00</t>
         </is>
       </c>
       <c r="E2" s="3" t="n">
@@ -584,12 +582,12 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>i-001b58faac5d5a771</t>
+          <t>i-0c5b84b6124fe0cea</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>jitsi-2</t>
+          <t>jibri</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
@@ -599,7 +597,7 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>2025-06-14 09:19:46+00:00</t>
+          <t>2025-06-17 04:33:12+00:00</t>
         </is>
       </c>
       <c r="E3" s="5" t="n">
@@ -617,6 +615,47 @@
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>Instance is stopped. Consider terminating if not needed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>i-0e31283df1ccc48fa</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>stopped</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>2025-06-17 04:43:57+00:00</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
         <is>
           <t>Instance is stopped. Consider terminating if not needed.</t>
         </is>
@@ -633,7 +672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -690,25 +729,25 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>snap-0864c1d6eadc4fcf3</t>
+          <t>snap-0779973fe6becea18</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>vol-0e1b8585e24d4f437</t>
+          <t>vol-024cceefe24c7f489</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>2025-06-12 14:52:07.626000+00:00</t>
+          <t>2025-06-17 04:46:15.715000+00:00</t>
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Created by CreateImage(i-06e22be674428fb8d) for ami-03fe541226ed7a78f</t>
+          <t>Created by CreateImage(i-0c5b84b6124fe0cea) for ami-0e104fa216390de2c</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -725,25 +764,25 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>snap-03cc57cae21173bf8</t>
+          <t>snap-06b556ee7de705219</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>vol-0ddfdc9b6e5f00562</t>
+          <t>vol-0a79835ead2f3b86b</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>2025-06-09 04:40:06.769000+00:00</t>
+          <t>2025-06-16 16:35:50.603000+00:00</t>
         </is>
       </c>
       <c r="D3" s="5" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="inlineStr">
         <is>
-          <t>Created by CreateImage(i-06c7ed8a4e83d47ae) for ami-0d1213ebe53bab3a3</t>
+          <t>Created by CreateImage(i-0ee13c6a8a2576a6d) for ami-0717f20c013e5c090</t>
         </is>
       </c>
       <c r="F3" s="5" t="inlineStr">
@@ -752,181 +791,6 @@
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>Delete if snapshot is orphan and not used by AMI or restore point.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>snap-0cfdb6658237d7d4d</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>vol-0c91412188bb749d7</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>2025-06-11 12:17:20.403000+00:00</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Created by CreateImage(i-09ad45b3c32ddfd36) for ami-0eb42d6e6d10db5d1</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>Delete if snapshot is orphan and not used by AMI or restore point.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>snap-0e3b1f133b9d7846b</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>vol-ffffffff</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>2025-06-05 07:10:50.025000+00:00</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5" t="inlineStr">
-        <is>
-          <t>Copied for DestinationAmi ami-0c757bca3918f6fa9 from SourceAmi ami-0eb5a8097071d95f9 for SourceSnapshot snap-01ce991a50576ecb7. Task created on 1,749,107,446,427.</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>Delete if snapshot is orphan and not used by AMI or restore point.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>snap-0a805599034e12c5b</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>vol-0203abc4a08c46aed</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>2025-06-15 03:57:21.744000+00:00</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>Created by CreateImage(i-001b58faac5d5a771) for ami-01b2b400e24fcdbe5</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>Delete if snapshot is orphan and not used by AMI or restore point.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>snap-033910e12c3e72780</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>vol-0abd53a95a3db1d6e</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>2025-06-11 12:16:28.682000+00:00</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>Created by CreateImage(i-03739429e37175531) for ami-0f84d671dcbc8a5e9</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>Delete if snapshot is orphan and not used by AMI or restore point.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>snap-06290303a513d7334</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>vol-0203abc4a08c46aed</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>2025-06-14 06:20:41.488000+00:00</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>Created by CreateImage(i-001b58faac5d5a771) for ami-0ef04d7a197cea5c8</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>Delete if snapshot is orphan and not used by AMI or restore point.</t>
         </is>
@@ -943,7 +807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,7 +829,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -982,22 +846,44 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>eni-0fdb33c06fd5cb15d</t>
+          <t>ami-0e104fa216390de2c</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>RDSNetworkInterface</t>
+          <t>jibri-setup</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Delete unattached ENI to avoid unnecessary charges.</t>
+          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>ami-0717f20c013e5c090</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>jitsi-insallation-image</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
         </is>
       </c>
     </row>
@@ -1007,207 +893,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Resource ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Used?</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Suggestion</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>ami-01b2b400e24fcdbe5</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>jitsi-2-latest</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>ami-0d1213ebe53bab3a3</t>
-        </is>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>jitsi-2</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>ami-0eb42d6e6d10db5d1</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>jitsi-5</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>ami-0ef04d7a197cea5c8</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>jitsi-2-official</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>ami-03fe541226ed7a78f</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>jitsi-final</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>ami-0c757bca3918f6fa9</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>jitsi</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>ami-0f84d671dcbc8a5e9</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>jitsi-4</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>Instance store-backed AMI. Check for leftover snapshots or data.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1327,7 +1012,7 @@
         <v>423</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>150.78</v>
+        <v>147.24</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>48</v>
@@ -1341,7 +1026,7 @@
       <c r="I2" s="3" t="inlineStr"/>
       <c r="J2" s="3" t="inlineStr"/>
       <c r="K2" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L2" s="3" t="n"/>
       <c r="M2" s="3" t="n"/>
@@ -1383,7 +1068,7 @@
       <c r="I3" s="5" t="inlineStr"/>
       <c r="J3" s="5" t="inlineStr"/>
       <c r="K3" s="5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L3" s="5" t="n"/>
       <c r="M3" s="5" t="n"/>
@@ -1411,10 +1096,10 @@
         <v>303</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>3406.82</v>
+        <v>3745.66</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3" t="b">
         <v>0</v>
@@ -1425,7 +1110,7 @@
       <c r="I4" s="3" t="inlineStr"/>
       <c r="J4" s="3" t="inlineStr"/>
       <c r="K4" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" s="3" t="n"/>
       <c r="M4" s="3" t="n"/>
@@ -1436,7 +1121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1654,7 +1339,7 @@
       </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
-          <t>No access logs or CloudTrail activity detected., Consider enabling object versioning.</t>
+          <t>No access logs or CloudTrail activity detected., No objects added in last 30 days., Consider enabling object versioning.</t>
         </is>
       </c>
     </row>
@@ -2199,11 +1884,11 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>0</v>
@@ -2231,32 +1916,6 @@
       <c r="J16" s="3" t="inlineStr">
         <is>
           <t>No access logs or CloudTrail activity detected., Consider enabling object versioning.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Invalid data format.</t>
         </is>
       </c>
     </row>

</xml_diff>